<commit_message>
better error handling, data validity checking
</commit_message>
<xml_diff>
--- a/assets/CanavanCalculator2.xlsx
+++ b/assets/CanavanCalculator2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbaumohl\Nextcloud\File_Sync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tech\Github\CanavanCalculator2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B708F282-122E-479F-A028-30A47AA533E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01AA26-2C97-4336-9556-9102FB062F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="87">
   <si>
     <t>%</t>
   </si>
@@ -284,13 +284,16 @@
     <t>Plate Appearance</t>
   </si>
   <si>
-    <t>Bazinga</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>Test Player</t>
+  </si>
+  <si>
+    <t>&lt;--- It's really Right Field for 9</t>
   </si>
 </sst>
 </file>
@@ -2187,20 +2190,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9B1455-5DA0-4BBC-8031-CAE08DC0431E}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.61328125" customWidth="1"/>
-    <col min="2" max="2" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.61328125" customWidth="1"/>
+    <col min="1" max="1" width="46.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.765625" customWidth="1"/>
+    <col min="8" max="8" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -2211,14 +2214,14 @@
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2232,7 +2235,7 @@
       <c r="I3" s="50"/>
       <c r="J3" s="50"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2248,7 +2251,7 @@
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2264,7 +2267,7 @@
       <c r="I5" s="50"/>
       <c r="J5" s="50"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2280,7 +2283,7 @@
       <c r="I6" s="50"/>
       <c r="J6" s="50"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2298,7 +2301,7 @@
       <c r="I7" s="50"/>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2316,7 +2319,7 @@
       <c r="I8" s="50"/>
       <c r="J8" s="50"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2334,7 +2337,7 @@
       <c r="I9" s="50"/>
       <c r="J9" s="50"/>
     </row>
-    <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F10" s="21" t="s">
         <v>16</v>
       </c>
@@ -2347,7 +2350,7 @@
       <c r="I10" s="50"/>
       <c r="J10" s="50"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F11" s="21" t="s">
         <v>17</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="I11" s="50"/>
       <c r="J11" s="50"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="F12" s="21" t="s">
         <v>15</v>
@@ -2372,7 +2375,7 @@
       <c r="I12" s="50"/>
       <c r="J12" s="50"/>
     </row>
-    <row r="13" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F13" s="22" t="s">
         <v>66</v>
       </c>
@@ -2385,7 +2388,7 @@
       <c r="I13" s="50"/>
       <c r="J13" s="50"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F14" s="21" t="s">
         <v>18</v>
       </c>
@@ -2396,7 +2399,7 @@
       <c r="I14" s="50"/>
       <c r="J14" s="50"/>
     </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
@@ -2416,7 +2419,7 @@
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -2436,7 +2439,7 @@
       <c r="Q20" s="19"/>
       <c r="R20" s="19"/>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -2448,15 +2451,17 @@
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="L21" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
       <c r="O21" s="19"/>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -2476,7 +2481,7 @@
       <c r="Q22" s="19"/>
       <c r="R22" s="19"/>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -2496,7 +2501,7 @@
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -2516,7 +2521,7 @@
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -2524,7 +2529,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -2532,7 +2537,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -2540,7 +2545,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -2549,7 +2554,13 @@
       <c r="F28" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H4:J4"/>
@@ -2558,11 +2569,6 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H8:J8"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2573,28 +2579,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276E0B33-A8DA-48BE-8BFF-768FA4D15B8A}">
   <dimension ref="A1:AB91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.3046875" customWidth="1"/>
-    <col min="3" max="3" width="5.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.23046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.23046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.296875" customWidth="1"/>
+    <col min="3" max="3" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C2" s="52" t="s">
         <v>39</v>
       </c>
@@ -2616,7 +2622,7 @@
       <c r="S2" s="53"/>
       <c r="T2" s="53"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
       <c r="E3" s="53"/>
@@ -2636,7 +2642,7 @@
       <c r="S3" s="53"/>
       <c r="T3" s="53"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C4" s="53"/>
       <c r="D4" s="53"/>
       <c r="E4" s="53"/>
@@ -2656,7 +2662,7 @@
       <c r="S4" s="53"/>
       <c r="T4" s="53"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C5" s="53"/>
       <c r="D5" s="53"/>
       <c r="E5" s="53"/>
@@ -2676,7 +2682,7 @@
       <c r="S5" s="53"/>
       <c r="T5" s="53"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
       <c r="E6" s="53"/>
@@ -2696,7 +2702,7 @@
       <c r="S6" s="53"/>
       <c r="T6" s="53"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
       <c r="E7" s="53"/>
@@ -2716,12 +2722,12 @@
       <c r="S7" s="53"/>
       <c r="T7" s="53"/>
     </row>
-    <row r="8" spans="1:28" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D8" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F8" s="51" t="s">
         <v>57</v>
@@ -2730,19 +2736,19 @@
       <c r="H8" s="51"/>
       <c r="I8" s="51"/>
     </row>
-    <row r="9" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:28" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="D12" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="13">
         <f ca="1">COUNTA(INDIRECT("'" &amp; $E$8 &amp; "'!B:B")) -1</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="25" t="s">
@@ -2821,7 +2827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>29</v>
       </c>
@@ -3036,13 +3042,13 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="14">
         <f ca="1">B15/$B$13</f>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="29">
@@ -3050,7 +3056,7 @@
       </c>
       <c r="E16" s="30">
         <f ca="1">COUNTIF(INDIRECT("'" &amp; $E$8 &amp; "'!E:E"),D16)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F16" s="31">
         <f ca="1">E16/$B$13</f>
@@ -3070,7 +3076,7 @@
       </c>
       <c r="J16" s="32">
         <f t="shared" ca="1" si="14"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="K16" s="30">
         <f t="shared" si="4"/>
@@ -3118,7 +3124,7 @@
       </c>
       <c r="V16" s="32">
         <f t="shared" ca="1" si="20"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W16" s="30">
         <f t="shared" si="10"/>
@@ -3145,7 +3151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>29</v>
       </c>
@@ -3269,7 +3275,7 @@
       </c>
       <c r="F18" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G18" s="30">
         <f t="shared" si="2"/>
@@ -3360,13 +3366,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="14">
         <f ca="1">B18/$B$13</f>
-        <v>0.3</v>
+        <v>0.75</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="29">
@@ -3378,7 +3384,7 @@
       </c>
       <c r="F19" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G19" s="30">
         <f t="shared" si="2"/>
@@ -3469,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>32</v>
       </c>
@@ -3501,7 +3507,7 @@
       <c r="AA20" s="35"/>
       <c r="AB20" s="35"/>
     </row>
-    <row r="21" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>29</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>30</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>33</v>
       </c>
@@ -3801,7 +3807,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>29</v>
       </c>
@@ -3910,7 +3916,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>30</v>
       </c>
@@ -4019,7 +4025,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>34</v>
       </c>
@@ -4125,7 +4131,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>29</v>
       </c>
@@ -4234,7 +4240,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>30</v>
       </c>
@@ -4343,7 +4349,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -4358,7 +4364,7 @@
       </c>
       <c r="F29" s="31">
         <f t="shared" ca="1" si="24"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G29" s="30">
         <f>COUNTIFS(INDIRECT("'" &amp; $E$8 &amp; "'!C:C"),2,INDIRECT("'" &amp; $E$8 &amp; "'!D:D"),1,INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$21)</f>
@@ -4449,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>29</v>
       </c>
@@ -4558,7 +4564,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>30</v>
       </c>
@@ -4667,7 +4673,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -4773,7 +4779,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>37</v>
       </c>
@@ -4791,7 +4797,7 @@
       </c>
       <c r="F33" s="31">
         <f t="shared" ca="1" si="24"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="30">
         <f>COUNTIFS(INDIRECT("'" &amp; $E$8 &amp; "'!C:C"),3,INDIRECT("'" &amp; $E$8 &amp; "'!D:D"),2,INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$21)</f>
@@ -4882,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>38</v>
       </c>
@@ -4917,9 +4923,9 @@
       <c r="AA34" s="35"/>
       <c r="AB34" s="35"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="13">
         <f>MODE(INDIRECT("'" &amp; $E$8 &amp; "'!E:E"))</f>
@@ -5002,9 +5008,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="12">
         <f>MEDIAN(INDIRECT("'" &amp; $E$8 &amp; "'!E:E"))</f>
@@ -5020,7 +5026,7 @@
       </c>
       <c r="F36" s="31">
         <f t="shared" ref="F36:F39" ca="1" si="134">E36/$B$13</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G36" s="30">
         <f>COUNTIFS(INDIRECT("'" &amp; $E$8 &amp; "'!F:F"),$D36,INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$35)</f>
@@ -5111,7 +5117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
@@ -5124,7 +5130,7 @@
       </c>
       <c r="F37" s="31">
         <f t="shared" ca="1" si="134"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G37" s="30">
         <f>COUNTIFS(INDIRECT("'" &amp; $E$8 &amp; "'!F:F"),$D37,INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$35)</f>
@@ -5215,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D38" s="29" t="s">
         <v>4</v>
       </c>
@@ -5316,7 +5322,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D39" s="29" t="s">
         <v>21</v>
       </c>
@@ -5326,7 +5332,7 @@
       </c>
       <c r="F39" s="31">
         <f t="shared" ca="1" si="134"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G39" s="30">
         <f>COUNTIFS(INDIRECT("'" &amp; $E$8 &amp; "'!F:F"),$D39,INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$35)</f>
@@ -5417,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
       <c r="D40" s="40"/>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
@@ -5444,7 +5450,7 @@
       <c r="AA40" s="35"/>
       <c r="AB40" s="35"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D41" s="25" t="s">
         <v>13</v>
       </c>
@@ -5521,7 +5527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D42" s="29">
         <v>0</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D43" s="29">
         <v>1</v>
       </c>
@@ -5723,7 +5729,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D44" s="29">
         <v>2</v>
       </c>
@@ -5824,7 +5830,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D45" s="29">
         <v>3</v>
       </c>
@@ -5925,7 +5931,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D46" s="29">
         <v>4</v>
       </c>
@@ -6026,7 +6032,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D47" s="29">
         <v>5</v>
       </c>
@@ -6127,7 +6133,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D48" s="29">
         <v>6</v>
       </c>
@@ -6228,7 +6234,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="49" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D49" s="29">
         <v>7</v>
       </c>
@@ -6329,7 +6335,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="50" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D50" s="29">
         <v>8</v>
       </c>
@@ -6430,7 +6436,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="51" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D51" s="29">
         <v>9</v>
       </c>
@@ -6440,7 +6446,7 @@
       </c>
       <c r="F51" s="31">
         <f t="shared" ca="1" si="174"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G51" s="30">
         <f t="shared" si="175"/>
@@ -6531,7 +6537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D52" s="29">
         <v>10</v>
       </c>
@@ -6541,7 +6547,7 @@
       </c>
       <c r="F52" s="31">
         <f t="shared" ca="1" si="174"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G52" s="30">
         <f t="shared" si="175"/>
@@ -6632,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D53" s="29">
         <v>11</v>
       </c>
@@ -6642,7 +6648,7 @@
       </c>
       <c r="F53" s="31">
         <f t="shared" ca="1" si="174"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G53" s="30">
         <f t="shared" si="175"/>
@@ -6733,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D54" s="29">
         <v>12</v>
       </c>
@@ -6834,7 +6840,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="55" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:28" ht="15.75" x14ac:dyDescent="0.2">
       <c r="D55" s="40"/>
       <c r="E55" s="30"/>
       <c r="F55" s="30"/>
@@ -6861,7 +6867,7 @@
       <c r="AA55" s="35"/>
       <c r="AB55" s="35"/>
     </row>
-    <row r="56" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D56" s="25" t="s">
         <v>17</v>
       </c>
@@ -6938,7 +6944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D57" s="29">
         <v>1</v>
       </c>
@@ -7009,7 +7015,7 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
     </row>
-    <row r="58" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D58" s="29">
         <v>2</v>
       </c>
@@ -7080,7 +7086,7 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
     </row>
-    <row r="59" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D59" s="29">
         <v>3</v>
       </c>
@@ -7151,7 +7157,7 @@
       <c r="AA59" s="43"/>
       <c r="AB59" s="43"/>
     </row>
-    <row r="60" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D60" s="29">
         <v>4</v>
       </c>
@@ -7222,7 +7228,7 @@
       <c r="AA60" s="43"/>
       <c r="AB60" s="43"/>
     </row>
-    <row r="61" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D61" s="29">
         <v>5</v>
       </c>
@@ -7232,7 +7238,7 @@
       </c>
       <c r="F61" s="31">
         <f t="shared" ca="1" si="330"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G61" s="30">
         <f t="shared" si="331"/>
@@ -7293,7 +7299,7 @@
       <c r="AA61" s="43"/>
       <c r="AB61" s="43"/>
     </row>
-    <row r="62" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D62" s="29">
         <v>6</v>
       </c>
@@ -7364,7 +7370,7 @@
       <c r="AA62" s="43"/>
       <c r="AB62" s="43"/>
     </row>
-    <row r="63" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D63" s="29">
         <v>7</v>
       </c>
@@ -7374,7 +7380,7 @@
       </c>
       <c r="F63" s="31">
         <f t="shared" ca="1" si="330"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G63" s="30">
         <f t="shared" si="331"/>
@@ -7435,7 +7441,7 @@
       <c r="AA63" s="43"/>
       <c r="AB63" s="43"/>
     </row>
-    <row r="64" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D64" s="29">
         <v>8</v>
       </c>
@@ -7445,7 +7451,7 @@
       </c>
       <c r="F64" s="31">
         <f t="shared" ca="1" si="330"/>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G64" s="30">
         <f t="shared" si="331"/>
@@ -7506,7 +7512,7 @@
       <c r="AA64" s="43"/>
       <c r="AB64" s="43"/>
     </row>
-    <row r="65" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D65" s="29">
         <v>9</v>
       </c>
@@ -7577,7 +7583,7 @@
       <c r="AA65" s="43"/>
       <c r="AB65" s="43"/>
     </row>
-    <row r="66" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D66" s="21"/>
       <c r="E66" s="35"/>
       <c r="F66" s="35"/>
@@ -7604,7 +7610,7 @@
       <c r="AA66" s="35"/>
       <c r="AB66" s="35"/>
     </row>
-    <row r="67" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D67" s="44" t="s">
         <v>56</v>
       </c>
@@ -7655,13 +7661,13 @@
       </c>
       <c r="AB67" s="21"/>
     </row>
-    <row r="68" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="21"/>
       <c r="G68" s="21">
         <f ca="1">COUNTIF(INDIRECT("'" &amp; $E$8 &amp; "'!H:H"),G$67)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H68" s="21"/>
       <c r="I68" s="21">
@@ -7715,10 +7721,10 @@
       </c>
       <c r="AB68" s="21"/>
     </row>
-    <row r="69" spans="4:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:28" x14ac:dyDescent="0.2">
       <c r="Y69" s="24"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
     </row>
@@ -7740,20 +7746,20 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.765625" style="48"/>
+    <col min="1" max="1" width="8.796875" style="48"/>
     <col min="2" max="2" width="11" style="48" customWidth="1"/>
-    <col min="3" max="7" width="8.765625" style="48"/>
-    <col min="8" max="8" width="17.3828125" style="48" customWidth="1"/>
-    <col min="9" max="9" width="8.765625" style="48"/>
-    <col min="10" max="10" width="8.23046875" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.765625" style="48"/>
+    <col min="3" max="7" width="8.796875" style="48"/>
+    <col min="8" max="8" width="17.3984375" style="48" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" style="48"/>
+    <col min="10" max="10" width="8.19921875" style="48" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="48"/>
     <col min="12" max="12" width="28" style="48" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.765625" style="48"/>
+    <col min="13" max="16384" width="8.796875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
@@ -7797,7 +7803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="48">
         <v>1</v>
       </c>
@@ -7829,7 +7835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="48">
         <v>2</v>
       </c>
@@ -7861,7 +7867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="48">
         <v>3</v>
       </c>
@@ -7893,7 +7899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="48">
         <v>4</v>
       </c>
@@ -7938,15 +7944,15 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="17.4609375" customWidth="1"/>
-    <col min="9" max="9" width="7.07421875" customWidth="1"/>
-    <col min="10" max="10" width="8.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="7.09765625" customWidth="1"/>
+    <col min="10" max="10" width="8.69921875" customWidth="1"/>
     <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -7990,7 +7996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
@@ -8022,7 +8028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
@@ -8054,7 +8060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
@@ -8086,7 +8092,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
@@ -8115,7 +8121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -8144,7 +8150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>6</v>
       </c>
@@ -8173,7 +8179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>7</v>
       </c>
@@ -8202,7 +8208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>8</v>
       </c>
@@ -8234,7 +8240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>9</v>
       </c>
@@ -8266,7 +8272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>10</v>
       </c>

</xml_diff>